<commit_message>
better arrange statistical tests
</commit_message>
<xml_diff>
--- a/fault_injection_mlaas/statistical_tests/summary_mannwhitneyu.xlsx
+++ b/fault_injection_mlaas/statistical_tests/summary_mannwhitneyu.xlsx
@@ -369,7 +369,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -422,9 +422,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -438,6 +435,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -948,8 +951,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A118" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A121" sqref="A121:G133"/>
+    <sheetView tabSelected="1" topLeftCell="A116" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A90" sqref="A90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -974,12 +977,12 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
@@ -1045,16 +1048,16 @@
       <c r="D9" s="8"/>
     </row>
     <row r="11" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="41" t="s">
+      <c r="A11" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="41"/>
-      <c r="C11" s="41"/>
-      <c r="D11" s="41"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
-      <c r="G11" s="41"/>
-      <c r="H11" s="41"/>
+      <c r="B11" s="40"/>
+      <c r="C11" s="40"/>
+      <c r="D11" s="40"/>
+      <c r="E11" s="40"/>
+      <c r="F11" s="40"/>
+      <c r="G11" s="40"/>
+      <c r="H11" s="40"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -2267,7 +2270,7 @@
       <c r="A78" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="B78" s="38">
+      <c r="B78" s="37">
         <v>2.605174426092086E-2</v>
       </c>
       <c r="C78" s="20">
@@ -2287,10 +2290,10 @@
       </c>
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A79" s="37" t="s">
+      <c r="A79" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="B79" s="39">
+      <c r="B79" s="38">
         <v>1.051852810641966E-2</v>
       </c>
       <c r="C79" s="24">
@@ -2310,7 +2313,7 @@
       </c>
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A80" s="37" t="s">
+      <c r="A80" s="36" t="s">
         <v>15</v>
       </c>
       <c r="B80" s="27">
@@ -2333,7 +2336,7 @@
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A81" s="37" t="s">
+      <c r="A81" s="36" t="s">
         <v>16</v>
       </c>
       <c r="B81" s="27">
@@ -2356,7 +2359,7 @@
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A82" s="37" t="s">
+      <c r="A82" s="36" t="s">
         <v>17</v>
       </c>
       <c r="B82" s="27">
@@ -2379,7 +2382,7 @@
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A83" s="37" t="s">
+      <c r="A83" s="36" t="s">
         <v>18</v>
       </c>
       <c r="B83" s="27">
@@ -2402,7 +2405,7 @@
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A84" s="37" t="s">
+      <c r="A84" s="36" t="s">
         <v>19</v>
       </c>
       <c r="B84" s="27">
@@ -2425,7 +2428,7 @@
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A85" s="37" t="s">
+      <c r="A85" s="36" t="s">
         <v>20</v>
       </c>
       <c r="B85" s="27">
@@ -2448,7 +2451,7 @@
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A86" s="37" t="s">
+      <c r="A86" s="36" t="s">
         <v>21</v>
       </c>
       <c r="B86" s="27">
@@ -2471,7 +2474,7 @@
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A87" s="37" t="s">
+      <c r="A87" s="36" t="s">
         <v>22</v>
       </c>
       <c r="B87" s="27">
@@ -2494,7 +2497,7 @@
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A88" s="37" t="s">
+      <c r="A88" s="36" t="s">
         <v>23</v>
       </c>
       <c r="B88" s="27">
@@ -2568,7 +2571,7 @@
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A94" s="28" t="s">
+      <c r="A94" s="42" t="s">
         <v>13</v>
       </c>
       <c r="B94" s="26">
@@ -2591,7 +2594,7 @@
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A95" s="28" t="s">
+      <c r="A95" s="42" t="s">
         <v>14</v>
       </c>
       <c r="B95" s="27">
@@ -2614,7 +2617,7 @@
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A96" s="28" t="s">
+      <c r="A96" s="42" t="s">
         <v>15</v>
       </c>
       <c r="B96" s="27">
@@ -2637,7 +2640,7 @@
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A97" s="28" t="s">
+      <c r="A97" s="42" t="s">
         <v>16</v>
       </c>
       <c r="B97" s="27">
@@ -2660,7 +2663,7 @@
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A98" s="28" t="s">
+      <c r="A98" s="42" t="s">
         <v>17</v>
       </c>
       <c r="B98" s="27">
@@ -2683,7 +2686,7 @@
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A99" s="28" t="s">
+      <c r="A99" s="42" t="s">
         <v>18</v>
       </c>
       <c r="B99" s="27">
@@ -2706,7 +2709,7 @@
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A100" s="28" t="s">
+      <c r="A100" s="42" t="s">
         <v>19</v>
       </c>
       <c r="B100" s="27">
@@ -2729,7 +2732,7 @@
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A101" s="28" t="s">
+      <c r="A101" s="42" t="s">
         <v>20</v>
       </c>
       <c r="B101" s="27">
@@ -2752,7 +2755,7 @@
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A102" s="28" t="s">
+      <c r="A102" s="42" t="s">
         <v>21</v>
       </c>
       <c r="B102" s="27">
@@ -2775,7 +2778,7 @@
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A103" s="28" t="s">
+      <c r="A103" s="42" t="s">
         <v>22</v>
       </c>
       <c r="B103" s="27">
@@ -2798,7 +2801,7 @@
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A104" s="28" t="s">
+      <c r="A104" s="42" t="s">
         <v>23</v>
       </c>
       <c r="B104" s="27">
@@ -2821,7 +2824,7 @@
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A105" s="28" t="s">
+      <c r="A105" s="42" t="s">
         <v>24</v>
       </c>
       <c r="B105" s="34">
@@ -3166,7 +3169,7 @@
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A122" s="36" t="s">
+      <c r="A122" s="43" t="s">
         <v>13</v>
       </c>
       <c r="B122" s="26">
@@ -3189,7 +3192,7 @@
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A123" s="28" t="s">
+      <c r="A123" s="42" t="s">
         <v>14</v>
       </c>
       <c r="B123" s="27">
@@ -3212,7 +3215,7 @@
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A124" s="28" t="s">
+      <c r="A124" s="42" t="s">
         <v>15</v>
       </c>
       <c r="B124" s="27">
@@ -3235,7 +3238,7 @@
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A125" s="28" t="s">
+      <c r="A125" s="42" t="s">
         <v>16</v>
       </c>
       <c r="B125" s="27">
@@ -3258,7 +3261,7 @@
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A126" s="28" t="s">
+      <c r="A126" s="42" t="s">
         <v>17</v>
       </c>
       <c r="B126" s="27">
@@ -3281,7 +3284,7 @@
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A127" s="28" t="s">
+      <c r="A127" s="42" t="s">
         <v>18</v>
       </c>
       <c r="B127" s="27">
@@ -3304,7 +3307,7 @@
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A128" s="28" t="s">
+      <c r="A128" s="42" t="s">
         <v>19</v>
       </c>
       <c r="B128" s="27">
@@ -3327,7 +3330,7 @@
       </c>
     </row>
     <row r="129" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A129" s="28" t="s">
+      <c r="A129" s="42" t="s">
         <v>20</v>
       </c>
       <c r="B129" s="27">
@@ -3350,7 +3353,7 @@
       </c>
     </row>
     <row r="130" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A130" s="28" t="s">
+      <c r="A130" s="42" t="s">
         <v>21</v>
       </c>
       <c r="B130" s="27">
@@ -3373,7 +3376,7 @@
       </c>
     </row>
     <row r="131" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A131" s="28" t="s">
+      <c r="A131" s="42" t="s">
         <v>22</v>
       </c>
       <c r="B131" s="27">
@@ -3396,7 +3399,7 @@
       </c>
     </row>
     <row r="132" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A132" s="28" t="s">
+      <c r="A132" s="42" t="s">
         <v>23</v>
       </c>
       <c r="B132" s="27">
@@ -3419,7 +3422,7 @@
       </c>
     </row>
     <row r="133" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A133" s="28" t="s">
+      <c r="A133" s="42" t="s">
         <v>24</v>
       </c>
       <c r="B133" s="34">
@@ -4022,15 +4025,15 @@
       </c>
     </row>
     <row r="152" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A152" s="42" t="s">
+      <c r="A152" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="B152" s="42"/>
-      <c r="C152" s="42"/>
-      <c r="D152" s="42"/>
-      <c r="E152" s="42"/>
-      <c r="F152" s="42"/>
-      <c r="G152" s="42"/>
+      <c r="B152" s="41"/>
+      <c r="C152" s="41"/>
+      <c r="D152" s="41"/>
+      <c r="E152" s="41"/>
+      <c r="F152" s="41"/>
+      <c r="G152" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>